<commit_message>
sync, created several networks
</commit_message>
<xml_diff>
--- a/ShapeNet/Results.xlsx
+++ b/ShapeNet/Results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="124">
   <si>
     <t xml:space="preserve">iou</t>
   </si>
@@ -264,7 +264,136 @@
     <t xml:space="preserve">Weighted average IOU is 0.838882</t>
   </si>
   <si>
+    <t xml:space="preserve">best+variance sacling+regularization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 22 trained in 416.028952, cost 113.340152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model saved in file: ./3d-object-recognition\ShapeNet\ShapeNet22.ckpt</t>
+  </si>
+  <si>
     <t xml:space="preserve">35GB train data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">train deconvolution average accuracy 0.957705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">train category accuracy 0.993248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluating train</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category airplane has 4 parts and IoU 0.826747</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category bag has 2 parts and IoU 0.808461</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category cap has 2 parts and IoU 0.916903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category car has 4 parts and IoU 0.791826</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category chair has 4 parts and IoU 0.911943</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category earphone has 3 parts and IoU 0.556492</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category guitar has 3 parts and IoU 0.881702</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category knife has 2 parts and IoU 0.844052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category lamp has 4 parts and IoU 0.870830</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category laptop has 2 parts and IoU 0.956305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category motorbike has 6 parts and IoU 0.556993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category mug has 2 parts and IoU 0.937098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category pistol has 3 parts and IoU 0.851671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category rocket has 3 parts and IoU 0.441905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category skateboard has 3 parts and IoU 0.730330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category table has 3 parts and IoU 0.861034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted average IOU is 0.860397</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dev deconvolution average accuracy 0.939193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dev category accuracy 0.989774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluating dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category airplane has 4 parts and IoU 0.833135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category bag has 2 parts and IoU 0.739287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category cap has 2 parts and IoU 0.542882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category car has 4 parts and IoU 0.777862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category chair has 4 parts and IoU 0.903612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category earphone has 3 parts and IoU 0.511505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category guitar has 3 parts and IoU 0.879616</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category knife has 2 parts and IoU 0.781302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category lamp has 4 parts and IoU 0.796643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category laptop has 2 parts and IoU 0.965612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category motorbike has 6 parts and IoU 0.525037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category mug has 2 parts and IoU 0.925973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category pistol has 3 parts and IoU 0.841207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category rocket has 3 parts and IoU 0.437171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category skateboard has 3 parts and IoU 0.631756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category table has 3 parts and IoU 0.836823</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted average IOU is 0.839242</t>
   </si>
 </sst>
 </file>
@@ -378,10 +507,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -957,6 +1086,9 @@
       <c r="D31" s="0" t="n">
         <v>95.95</v>
       </c>
+      <c r="I31" s="0" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="n">
@@ -965,6 +1097,9 @@
       <c r="D32" s="0" t="n">
         <v>97.16</v>
       </c>
+      <c r="I32" s="0" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="n">
@@ -973,6 +1108,9 @@
       <c r="D33" s="0" t="n">
         <v>98.23</v>
       </c>
+      <c r="I33" s="0" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="n">
@@ -982,7 +1120,205 @@
         <v>99.78</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I35" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I36" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I37" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I38" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I39" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I40" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I41" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I42" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I43" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I44" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I45" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I46" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I47" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I48" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I49" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I50" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I51" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I52" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I53" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I54" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I55" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I56" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I57" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I58" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I59" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I60" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I61" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I62" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I63" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I64" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I65" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I66" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I67" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I68" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I69" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I70" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I71" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I72" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I73" s="0" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>